<commit_message>
inverted y-axis and added the live data to plot
</commit_message>
<xml_diff>
--- a/data/preloaded_data/updated_well_data.xlsx
+++ b/data/preloaded_data/updated_well_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S.KARKI\Documents\2021\CSISA\gw-dashboard\groundwater_monitoring\data\preloaded_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0D773F5B-FAD8-4C9B-A74D-797A9B69A0B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248304F6-9BA2-4D89-A70B-43C976822EF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shallow Tube Wells" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="137">
   <si>
     <t xml:space="preserve">1-045/46(BK)1 </t>
   </si>
@@ -299,9 +299,6 @@
     <t>Well No.</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t xml:space="preserve">Location </t>
   </si>
   <si>
@@ -309,12 +306,138 @@
   </si>
   <si>
     <t>Latitude</t>
+  </si>
+  <si>
+    <t>bk-dw-01</t>
+  </si>
+  <si>
+    <t>bk-dw-02</t>
+  </si>
+  <si>
+    <t>bk-dw-03</t>
+  </si>
+  <si>
+    <t>bk-dw-04_1</t>
+  </si>
+  <si>
+    <t>bk-dw-05</t>
+  </si>
+  <si>
+    <t>bk-sw-01</t>
+  </si>
+  <si>
+    <t>bk-sw-02</t>
+  </si>
+  <si>
+    <t>bk-sw-03</t>
+  </si>
+  <si>
+    <t>bk-sw-04</t>
+  </si>
+  <si>
+    <t>bk-sw-05_1</t>
+  </si>
+  <si>
+    <t>bk-sw-06_1</t>
+  </si>
+  <si>
+    <t>bk-sw-07_1</t>
+  </si>
+  <si>
+    <t>bk-sw-08_1</t>
+  </si>
+  <si>
+    <t>bk-sw-09_1</t>
+  </si>
+  <si>
+    <t>bk-sw-10_1</t>
+  </si>
+  <si>
+    <t>bk-sw-11_1</t>
+  </si>
+  <si>
+    <t>bk-sw-12_1</t>
+  </si>
+  <si>
+    <t>bk-sw-13_1</t>
+  </si>
+  <si>
+    <t>bk-sw-14_1</t>
+  </si>
+  <si>
+    <t>bk-sw-15_1</t>
+  </si>
+  <si>
+    <t>bk-sw-16_1</t>
+  </si>
+  <si>
+    <t>bk-sw-17_1</t>
+  </si>
+  <si>
+    <t>bk-sw-18_1</t>
+  </si>
+  <si>
+    <t>bk-sw-19_1</t>
+  </si>
+  <si>
+    <t>bk-sw-20_1</t>
+  </si>
+  <si>
+    <t>bk-sw-21_1</t>
+  </si>
+  <si>
+    <t>bk-sw-22_1</t>
+  </si>
+  <si>
+    <t>bk-sw-23_1</t>
+  </si>
+  <si>
+    <t>bk-sw-24_1</t>
+  </si>
+  <si>
+    <t>bk-sw-25_1</t>
+  </si>
+  <si>
+    <t>bk-sw-26</t>
+  </si>
+  <si>
+    <t>bk-sw-27</t>
+  </si>
+  <si>
+    <t>well_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Matehiya</t>
+  </si>
+  <si>
+    <t>Bahartha</t>
+  </si>
+  <si>
+    <t>Narayanpur</t>
+  </si>
+  <si>
+    <t>Majharatriya</t>
+  </si>
+  <si>
+    <t>Rajgarhwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Balapur</t>
+  </si>
+  <si>
+    <t>Kachanapur</t>
+  </si>
+  <si>
+    <t>Binauna</t>
+  </si>
+  <si>
+    <t>Parspur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1148,11 +1271,796 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>81.516599999999997</v>
+      </c>
+      <c r="F2">
+        <v>28.122309999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>81.644302490000001</v>
+      </c>
+      <c r="F3">
+        <v>28.255733159999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>81.626708669999999</v>
+      </c>
+      <c r="F4">
+        <v>28.210681510000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>81.624591940000002</v>
+      </c>
+      <c r="F5">
+        <v>28.197151099999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>81.583815250000001</v>
+      </c>
+      <c r="F6">
+        <v>28.193269059999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>81.659897380000004</v>
+      </c>
+      <c r="F7">
+        <v>28.13921427</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>81.632117160000007</v>
+      </c>
+      <c r="F8">
+        <v>28.090600290000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>81.660373989999997</v>
+      </c>
+      <c r="F9">
+        <v>28.050748980000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>81.667284640000005</v>
+      </c>
+      <c r="F10">
+        <v>28.016413320000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>81.719469410000002</v>
+      </c>
+      <c r="F11">
+        <v>27.986361299999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>81.601249870000004</v>
+      </c>
+      <c r="F12">
+        <v>28.031161239999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18">
+        <v>81.611090180000005</v>
+      </c>
+      <c r="F18">
+        <v>28.15207814</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19">
+        <v>81.55200198</v>
+      </c>
+      <c r="F19">
+        <v>28.148718200000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20">
+        <v>81.555842749999996</v>
+      </c>
+      <c r="F20">
+        <v>28.103568200000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21">
+        <v>81.756057749999997</v>
+      </c>
+      <c r="F21">
+        <v>28.201452629999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>81.645009999999999</v>
+      </c>
+      <c r="F25">
+        <v>28.081250000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>81.798199999999994</v>
+      </c>
+      <c r="F26">
+        <v>28.14303</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27">
+        <v>81.593260000000001</v>
+      </c>
+      <c r="F27">
+        <v>28.07807</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28">
+        <v>81.595560000000006</v>
+      </c>
+      <c r="F28">
+        <v>28.08276</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,16 +2073,16 @@
         <v>91</v>
       </c>
       <c r="C1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>94</v>
-      </c>
-      <c r="F1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1182,16 +2090,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="E2">
-        <v>81.516599999999997</v>
+        <v>81.645009999999999</v>
       </c>
       <c r="F2">
-        <v>28.122309999999999</v>
+        <v>28.081250000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1199,16 +2110,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="E3">
-        <v>81.644302490000001</v>
+        <v>81.798199999999994</v>
       </c>
       <c r="F3">
-        <v>28.255733159999998</v>
+        <v>28.14303</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1216,16 +2130,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="E4">
-        <v>81.626708669999999</v>
+        <v>81.593260000000001</v>
       </c>
       <c r="F4">
-        <v>28.210681510000001</v>
+        <v>28.07807</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1233,16 +2150,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E5">
-        <v>81.624591940000002</v>
+        <v>81.595560000000006</v>
       </c>
       <c r="F5">
-        <v>28.197151099999999</v>
+        <v>28.08276</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1250,16 +2170,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>99</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>81.583815250000001</v>
-      </c>
-      <c r="F6">
-        <v>28.193269059999999</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1267,16 +2184,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <v>81.659897380000004</v>
-      </c>
-      <c r="F7">
-        <v>28.13921427</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1284,16 +2195,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8">
-        <v>81.632117160000007</v>
-      </c>
-      <c r="F8">
-        <v>28.090600290000001</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1301,16 +2206,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <v>81.660373989999997</v>
-      </c>
-      <c r="F9">
-        <v>28.050748980000002</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1318,585 +2217,9 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10">
-        <v>81.667284640000005</v>
-      </c>
-      <c r="F10">
-        <v>28.016413320000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11">
-        <v>81.719469410000002</v>
-      </c>
-      <c r="F11">
-        <v>27.986361299999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12">
-        <v>81.601249870000004</v>
-      </c>
-      <c r="F12">
-        <v>28.031161239999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13">
-        <v>81.611090180000005</v>
-      </c>
-      <c r="F13">
-        <v>28.15207814</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14">
-        <v>81.55200198</v>
-      </c>
-      <c r="F14">
-        <v>28.148718200000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15">
-        <v>81.555842749999996</v>
-      </c>
-      <c r="F15">
-        <v>28.103568200000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16">
-        <v>81.756057749999997</v>
-      </c>
-      <c r="F16">
-        <v>28.201452629999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17">
-        <v>81.645009999999999</v>
-      </c>
-      <c r="F17">
-        <v>28.081250000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18">
-        <v>81.798199999999994</v>
-      </c>
-      <c r="F18">
-        <v>28.14303</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19">
-        <v>81.593260000000001</v>
-      </c>
-      <c r="F19">
-        <v>28.07807</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20">
-        <v>81.595560000000006</v>
-      </c>
-      <c r="F20">
-        <v>28.08276</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>4</v>
-      </c>
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>6</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>8</v>
-      </c>
-      <c r="B28" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>9</v>
-      </c>
-      <c r="B29" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>10</v>
-      </c>
-      <c r="B30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>11</v>
-      </c>
-      <c r="B31" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>12</v>
-      </c>
-      <c r="B32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>13</v>
-      </c>
-      <c r="B33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>14</v>
-      </c>
-      <c r="B34" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>15</v>
-      </c>
-      <c r="B35" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>16</v>
-      </c>
-      <c r="B36" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>17</v>
-      </c>
-      <c r="B37" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>18</v>
-      </c>
-      <c r="B38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>19</v>
-      </c>
-      <c r="B39" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>20</v>
-      </c>
-      <c r="B40" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>21</v>
-      </c>
-      <c r="B41" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>22</v>
-      </c>
-      <c r="B42" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>23</v>
-      </c>
-      <c r="B43" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2">
-        <v>81.645009999999999</v>
-      </c>
-      <c r="F2">
-        <v>28.081250000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3">
-        <v>81.798199999999994</v>
-      </c>
-      <c r="F3">
-        <v>28.14303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4">
-        <v>81.593260000000001</v>
-      </c>
-      <c r="F4">
-        <v>28.07807</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5">
-        <v>81.595560000000006</v>
-      </c>
-      <c r="F5">
-        <v>28.08276</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
making changes to map
</commit_message>
<xml_diff>
--- a/data/preloaded_data/updated_well_data.xlsx
+++ b/data/preloaded_data/updated_well_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S.KARKI\Documents\2021\CSISA\gw-dashboard\groundwater_monitoring\data\preloaded_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248304F6-9BA2-4D89-A70B-43C976822EF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420FE620-85DE-4561-8171-AAA032B91B57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1274,12 +1274,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="10" max="11" width="9.140625" customWidth="1"/>

</xml_diff>

<commit_message>
updated well location gps
</commit_message>
<xml_diff>
--- a/data/preloaded_data/updated_well_data.xlsx
+++ b/data/preloaded_data/updated_well_data.xlsx
@@ -1,33 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S.KARKI\Documents\2021\CSISA\gw-dashboard\groundwater_monitoring\data\preloaded_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saralkarki/Documents/projects/gw_dash/groundwater_monitoring/data/preloaded_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F19BC3B-D6D9-4798-87B2-0C97070A24D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAF53F5-09F4-8941-99F5-6B66673774FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shallow Tube Wells" sheetId="2" r:id="rId1"/>
     <sheet name="Deep tube wells" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1351,19 +1340,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="9" max="10" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -1386,7 +1375,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1400,16 +1389,16 @@
         <v>120</v>
       </c>
       <c r="E2">
-        <v>81.516599999999997</v>
+        <v>81.641929300000001</v>
       </c>
       <c r="F2">
-        <v>28.122309999999999</v>
+        <v>28.080494300000002</v>
       </c>
       <c r="G2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1423,16 +1412,16 @@
         <v>121</v>
       </c>
       <c r="E3">
-        <v>81.644302490000001</v>
+        <v>81.636181899999997</v>
       </c>
       <c r="F3">
-        <v>28.255733159999998</v>
+        <v>28.2576903</v>
       </c>
       <c r="G3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1446,16 +1435,16 @@
         <v>122</v>
       </c>
       <c r="E4">
-        <v>81.626708669999999</v>
+        <v>81.6307264</v>
       </c>
       <c r="F4">
-        <v>28.210681510000001</v>
+        <v>28.206494899999999</v>
       </c>
       <c r="G4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1469,16 +1458,16 @@
         <v>123</v>
       </c>
       <c r="E5">
-        <v>81.624591940000002</v>
+        <v>81.6300983</v>
       </c>
       <c r="F5">
-        <v>28.197151099999999</v>
+        <v>28.1873921</v>
       </c>
       <c r="G5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1492,16 +1481,16 @@
         <v>124</v>
       </c>
       <c r="E6">
-        <v>81.583815250000001</v>
+        <v>81.574748099999994</v>
       </c>
       <c r="F6">
-        <v>28.193269059999999</v>
+        <v>28.192045499999999</v>
       </c>
       <c r="G6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1515,16 +1504,16 @@
         <v>125</v>
       </c>
       <c r="E7">
-        <v>81.659897380000004</v>
+        <v>81.658814599999999</v>
       </c>
       <c r="F7">
-        <v>28.13921427</v>
+        <v>28.131810000000002</v>
       </c>
       <c r="G7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1538,16 +1527,16 @@
         <v>126</v>
       </c>
       <c r="E8">
-        <v>81.632117160000007</v>
+        <v>81.647869299999996</v>
       </c>
       <c r="F8">
-        <v>28.090600290000001</v>
+        <v>28.092858199999998</v>
       </c>
       <c r="G8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1561,16 +1550,16 @@
         <v>127</v>
       </c>
       <c r="E9">
-        <v>81.660373989999997</v>
+        <v>81.661625799999996</v>
       </c>
       <c r="F9">
-        <v>28.050748980000002</v>
+        <v>28.049327399999999</v>
       </c>
       <c r="G9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1584,16 +1573,16 @@
         <v>128</v>
       </c>
       <c r="E10">
-        <v>81.667284640000005</v>
+        <v>81.654347900000005</v>
       </c>
       <c r="F10">
-        <v>28.016413320000002</v>
+        <v>28.015118300000001</v>
       </c>
       <c r="G10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1607,16 +1596,16 @@
         <v>129</v>
       </c>
       <c r="E11">
-        <v>81.719469410000002</v>
+        <v>81.713292300000006</v>
       </c>
       <c r="F11">
-        <v>27.986361299999999</v>
+        <v>27.983303899999999</v>
       </c>
       <c r="G11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1630,16 +1619,16 @@
         <v>130</v>
       </c>
       <c r="E12">
-        <v>81.601249870000004</v>
+        <v>81.600283599999997</v>
       </c>
       <c r="F12">
-        <v>28.031161239999999</v>
+        <v>28.024258700000001</v>
       </c>
       <c r="G12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>17</v>
       </c>
@@ -1653,16 +1642,16 @@
         <v>131</v>
       </c>
       <c r="E13">
-        <v>81.611090180000005</v>
+        <v>81.589428100000006</v>
       </c>
       <c r="F13">
-        <v>28.15207814</v>
+        <v>28.128715100000001</v>
       </c>
       <c r="G13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>18</v>
       </c>
@@ -1676,16 +1665,16 @@
         <v>132</v>
       </c>
       <c r="E14">
-        <v>81.55200198</v>
+        <v>81.551986200000002</v>
       </c>
       <c r="F14">
-        <v>28.148718200000001</v>
+        <v>28.146545400000001</v>
       </c>
       <c r="G14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>19</v>
       </c>
@@ -1699,16 +1688,16 @@
         <v>24</v>
       </c>
       <c r="E15">
-        <v>81.555842749999996</v>
+        <v>81.521693499999998</v>
       </c>
       <c r="F15">
-        <v>28.103568200000002</v>
+        <v>28.111447900000002</v>
       </c>
       <c r="G15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20</v>
       </c>
@@ -1731,7 +1720,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>24</v>
       </c>
@@ -1745,16 +1734,16 @@
         <v>134</v>
       </c>
       <c r="E17">
-        <v>81.645009999999999</v>
+        <v>81.645064300000001</v>
       </c>
       <c r="F17">
-        <v>28.081250000000001</v>
+        <v>28.081222400000001</v>
       </c>
       <c r="G17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>25</v>
       </c>
@@ -1768,16 +1757,16 @@
         <v>135</v>
       </c>
       <c r="E18">
-        <v>81.798199999999994</v>
+        <v>81.597155099999995</v>
       </c>
       <c r="F18">
-        <v>28.14303</v>
+        <v>28.106038600000002</v>
       </c>
       <c r="G18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>26</v>
       </c>
@@ -1791,16 +1780,16 @@
         <v>118</v>
       </c>
       <c r="E19">
-        <v>81.593260000000001</v>
+        <v>81.5933074</v>
       </c>
       <c r="F19">
-        <v>28.07807</v>
+        <v>28.0780663</v>
       </c>
       <c r="G19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>27</v>
       </c>
@@ -1814,16 +1803,16 @@
         <v>117</v>
       </c>
       <c r="E20">
-        <v>81.595560000000006</v>
+        <v>81.595679500000003</v>
       </c>
       <c r="F20">
-        <v>28.08276</v>
+        <v>28.082843700000002</v>
       </c>
       <c r="G20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>28</v>
       </c>
@@ -1836,11 +1825,17 @@
       <c r="D21" t="s">
         <v>114</v>
       </c>
+      <c r="E21">
+        <v>81.586179400000006</v>
+      </c>
+      <c r="F21">
+        <v>28.050744300000002</v>
+      </c>
       <c r="G21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>29</v>
       </c>
@@ -1853,11 +1848,17 @@
       <c r="D22" t="s">
         <v>115</v>
       </c>
+      <c r="E22">
+        <v>81.652378600000006</v>
+      </c>
+      <c r="F22">
+        <v>28.0020439</v>
+      </c>
       <c r="G22" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>30</v>
       </c>
@@ -1870,11 +1871,17 @@
       <c r="D23" t="s">
         <v>116</v>
       </c>
+      <c r="E23">
+        <v>81.694684800000005</v>
+      </c>
+      <c r="F23">
+        <v>28.0285434</v>
+      </c>
       <c r="G23" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>28</v>
       </c>
@@ -1887,11 +1894,17 @@
       <c r="D24" t="s">
         <v>136</v>
       </c>
+      <c r="E24">
+        <v>81.642070000000004</v>
+      </c>
+      <c r="F24">
+        <v>28.080324099999999</v>
+      </c>
       <c r="G24" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>29</v>
       </c>
@@ -1904,11 +1917,17 @@
       <c r="D25" t="s">
         <v>137</v>
       </c>
+      <c r="E25">
+        <v>81.547736200000003</v>
+      </c>
+      <c r="F25">
+        <v>28.236479299999999</v>
+      </c>
       <c r="G25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>30</v>
       </c>
@@ -1921,11 +1940,17 @@
       <c r="D26" t="s">
         <v>138</v>
       </c>
+      <c r="E26">
+        <v>81.479971000000006</v>
+      </c>
+      <c r="F26">
+        <v>28.188046700000001</v>
+      </c>
       <c r="G26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>31</v>
       </c>
@@ -1938,11 +1963,17 @@
       <c r="D27" t="s">
         <v>139</v>
       </c>
+      <c r="E27">
+        <v>81.442083600000004</v>
+      </c>
+      <c r="F27">
+        <v>28.289843000000001</v>
+      </c>
       <c r="G27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>32</v>
       </c>
@@ -1955,11 +1986,17 @@
       <c r="D28" t="s">
         <v>140</v>
       </c>
+      <c r="E28">
+        <v>81.383682300000004</v>
+      </c>
+      <c r="F28">
+        <v>28.189743</v>
+      </c>
       <c r="G28" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>33</v>
       </c>
@@ -1972,11 +2009,17 @@
       <c r="D29" t="s">
         <v>141</v>
       </c>
+      <c r="E29">
+        <v>81.337879799999996</v>
+      </c>
+      <c r="F29">
+        <v>28.169159400000002</v>
+      </c>
       <c r="G29" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>34</v>
       </c>
@@ -1989,11 +2032,17 @@
       <c r="D30" t="s">
         <v>142</v>
       </c>
+      <c r="E30">
+        <v>81.359306799999999</v>
+      </c>
+      <c r="F30">
+        <v>28.305615700000001</v>
+      </c>
       <c r="G30" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>35</v>
       </c>
@@ -2006,11 +2055,17 @@
       <c r="D31" t="s">
         <v>143</v>
       </c>
+      <c r="E31">
+        <v>81.429742700000006</v>
+      </c>
+      <c r="F31">
+        <v>28.351235599999999</v>
+      </c>
       <c r="G31" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>36</v>
       </c>
@@ -2023,11 +2078,17 @@
       <c r="D32" t="s">
         <v>144</v>
       </c>
+      <c r="E32">
+        <v>81.310765599999996</v>
+      </c>
+      <c r="F32">
+        <v>28.250470400000001</v>
+      </c>
       <c r="G32" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>37</v>
       </c>
@@ -2040,11 +2101,17 @@
       <c r="D33" t="s">
         <v>145</v>
       </c>
+      <c r="E33">
+        <v>81.336589599999996</v>
+      </c>
+      <c r="F33">
+        <v>28.301372000000001</v>
+      </c>
       <c r="G33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>38</v>
       </c>
@@ -2057,11 +2124,17 @@
       <c r="D34" t="s">
         <v>146</v>
       </c>
+      <c r="E34">
+        <v>81.359149099999996</v>
+      </c>
+      <c r="F34">
+        <v>28.306523500000001</v>
+      </c>
       <c r="G34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>39</v>
       </c>
@@ -2074,11 +2147,17 @@
       <c r="D35" t="s">
         <v>147</v>
       </c>
+      <c r="E35">
+        <v>81.262822499999999</v>
+      </c>
+      <c r="F35">
+        <v>28.279571099999998</v>
+      </c>
       <c r="G35" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>40</v>
       </c>
@@ -2091,11 +2170,17 @@
       <c r="D36" t="s">
         <v>148</v>
       </c>
+      <c r="E36">
+        <v>81.266078399999998</v>
+      </c>
+      <c r="F36">
+        <v>28.3349604</v>
+      </c>
       <c r="G36" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>41</v>
       </c>
@@ -2108,11 +2193,17 @@
       <c r="D37" t="s">
         <v>149</v>
       </c>
+      <c r="E37">
+        <v>81.5542272</v>
+      </c>
+      <c r="F37">
+        <v>28.0731407</v>
+      </c>
       <c r="G37" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>42</v>
       </c>
@@ -2125,11 +2216,17 @@
       <c r="D38" t="s">
         <v>150</v>
       </c>
+      <c r="E38">
+        <v>81.554246300000003</v>
+      </c>
+      <c r="F38">
+        <v>28.073109800000001</v>
+      </c>
       <c r="G38" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>43</v>
       </c>
@@ -2142,11 +2239,17 @@
       <c r="D39" t="s">
         <v>151</v>
       </c>
+      <c r="E39">
+        <v>81.554121199999997</v>
+      </c>
+      <c r="F39">
+        <v>28.073126999999999</v>
+      </c>
       <c r="G39" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>44</v>
       </c>
@@ -2163,7 +2266,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>45</v>
       </c>
@@ -2176,11 +2279,17 @@
       <c r="D41" t="s">
         <v>153</v>
       </c>
+      <c r="E41">
+        <v>81.496865299999996</v>
+      </c>
+      <c r="F41">
+        <v>28.148684500000002</v>
+      </c>
       <c r="G41" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>46</v>
       </c>
@@ -2193,11 +2302,17 @@
       <c r="D42" t="s">
         <v>154</v>
       </c>
+      <c r="E42">
+        <v>81.479091499999996</v>
+      </c>
+      <c r="F42">
+        <v>28.146412300000001</v>
+      </c>
       <c r="G42" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>47</v>
       </c>
@@ -2210,11 +2325,17 @@
       <c r="D43" t="s">
         <v>153</v>
       </c>
+      <c r="E43">
+        <v>81.500847300000004</v>
+      </c>
+      <c r="F43">
+        <v>28.1656409</v>
+      </c>
       <c r="G43" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>48</v>
       </c>
@@ -2227,11 +2348,17 @@
       <c r="D44" t="s">
         <v>155</v>
       </c>
+      <c r="E44">
+        <v>81.567171200000004</v>
+      </c>
+      <c r="F44">
+        <v>28.2282732</v>
+      </c>
       <c r="G44" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>49</v>
       </c>
@@ -2244,11 +2371,17 @@
       <c r="D45" t="s">
         <v>155</v>
       </c>
+      <c r="E45">
+        <v>81.584886499999996</v>
+      </c>
+      <c r="F45">
+        <v>28.249013099999999</v>
+      </c>
       <c r="G45" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>50</v>
       </c>
@@ -2260,6 +2393,12 @@
       </c>
       <c r="D46" t="s">
         <v>156</v>
+      </c>
+      <c r="E46">
+        <v>81.288935100000003</v>
+      </c>
+      <c r="F46">
+        <v>28.238539500000002</v>
       </c>
       <c r="G46" t="s">
         <v>82</v>
@@ -2275,13 +2414,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -2304,7 +2443,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2318,16 +2457,16 @@
         <v>20</v>
       </c>
       <c r="E2">
-        <v>81.645009999999999</v>
+        <v>81.5466409</v>
       </c>
       <c r="F2">
-        <v>28.081250000000001</v>
+        <v>28.0818215</v>
       </c>
       <c r="G2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2341,16 +2480,16 @@
         <v>22</v>
       </c>
       <c r="E3">
-        <v>81.798199999999994</v>
+        <v>81.521136299999995</v>
       </c>
       <c r="F3">
-        <v>28.14303</v>
+        <v>28.096043600000002</v>
       </c>
       <c r="G3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2364,16 +2503,16 @@
         <v>24</v>
       </c>
       <c r="E4">
-        <v>81.593260000000001</v>
+        <v>81.5165796</v>
       </c>
       <c r="F4">
-        <v>28.07807</v>
+        <v>28.122328100000001</v>
       </c>
       <c r="G4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2387,16 +2526,16 @@
         <v>24</v>
       </c>
       <c r="E5">
-        <v>81.595560000000006</v>
+        <v>81.517303499999997</v>
       </c>
       <c r="F5">
-        <v>28.08276</v>
+        <v>28.113236100000002</v>
       </c>
       <c r="G5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2409,11 +2548,17 @@
       <c r="D6" t="s">
         <v>79</v>
       </c>
+      <c r="E6">
+        <v>81.602454100000003</v>
+      </c>
+      <c r="F6">
+        <v>28.0513081</v>
+      </c>
       <c r="G6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2426,11 +2571,17 @@
       <c r="D7" t="s">
         <v>48</v>
       </c>
+      <c r="E7">
+        <v>81.516361599999996</v>
+      </c>
+      <c r="F7">
+        <v>28.085180999999999</v>
+      </c>
       <c r="G7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2443,11 +2594,17 @@
       <c r="D8" t="s">
         <v>49</v>
       </c>
+      <c r="E8">
+        <v>81.482591299999996</v>
+      </c>
+      <c r="F8">
+        <v>28.105589899999998</v>
+      </c>
       <c r="G8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2460,11 +2617,17 @@
       <c r="D9" t="s">
         <v>48</v>
       </c>
+      <c r="E9">
+        <v>81.502630999999994</v>
+      </c>
+      <c r="F9">
+        <v>28.088340599999999</v>
+      </c>
       <c r="G9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2476,6 +2639,12 @@
       </c>
       <c r="D10" t="s">
         <v>48</v>
+      </c>
+      <c r="E10">
+        <v>81.511170800000002</v>
+      </c>
+      <c r="F10">
+        <v>28.082853100000001</v>
       </c>
       <c r="G10" t="s">
         <v>82</v>

</xml_diff>